<commit_message>
updated material for CIDR submission
</commit_message>
<xml_diff>
--- a/Pandas APIs Translatability.xlsx
+++ b/Pandas APIs Translatability.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/kvemani_microsoft_com/Documents/pyfroid_vldb2023_submission_material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvemani\datadrive\pyfroid_material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{74843531-A0CF-4119-8AF0-CCCEF5B65155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9C0FC42-85DB-47A7-B45F-3F39880BCCA8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C730C45-6BAA-4B6B-A696-93D6EF956DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5A1E631A-4991-4B3C-A0B0-668D66A578F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5A1E631A-4991-4B3C-A0B0-668D66A578F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Pandas APIs" sheetId="1" r:id="rId1"/>
+    <sheet name="GitHub data analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="239">
   <si>
     <t>DataFrame</t>
   </si>
@@ -749,6 +750,9 @@
   </si>
   <si>
     <t>Index related</t>
+  </si>
+  <si>
+    <t>Available on request. Please contact kvemani@microsoft.com</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8816E9F6-F121-4BB3-8A4A-381124A6926B}">
   <dimension ref="A1:K227"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C227" sqref="C227"/>
     </sheetView>
@@ -3595,6 +3599,27 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5559C0-B698-4044-82D3-0CE54DD033F2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="52.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>